<commit_message>
BHEL purchased and all decimals removed except loss or gain %
</commit_message>
<xml_diff>
--- a/stock_portfolio_report.xlsx
+++ b/stock_portfolio_report.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>160718.45</v>
+        <v>161424.2</v>
       </c>
       <c r="C2" t="n">
-        <v>170123.8584289551</v>
+        <v>170867.7984161377</v>
       </c>
       <c r="D2" t="n">
-        <v>9405.408428955066</v>
+        <v>9443.598416137684</v>
       </c>
       <c r="E2" t="n">
-        <v>5.852102499093953</v>
+        <v>5.850175138633293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
indian bank re updated to remove error on 06-11-2024 2203hrs
</commit_message>
<xml_diff>
--- a/stock_portfolio_report.xlsx
+++ b/stock_portfolio_report.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>228848.7</v>
+        <v>228777.2</v>
       </c>
       <c r="C2" t="n">
         <v>253157.1501617432</v>
       </c>
       <c r="D2" t="n">
-        <v>24308.45016174315</v>
+        <v>24379.95016174315</v>
       </c>
       <c r="E2" t="n">
-        <v>10.62206172101618</v>
+        <v>10.65663456049954</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added column profit booking
</commit_message>
<xml_diff>
--- a/stock_portfolio_report.xlsx
+++ b/stock_portfolio_report.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>228777.2</v>
+        <v>233673.2</v>
       </c>
       <c r="C2" t="n">
-        <v>253157.1501617432</v>
+        <v>258116.7500762939</v>
       </c>
       <c r="D2" t="n">
-        <v>24379.95016174315</v>
+        <v>24443.55007629396</v>
       </c>
       <c r="E2" t="n">
-        <v>10.65663456049954</v>
+        <v>10.46057060728144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
52 week high and low added
</commit_message>
<xml_diff>
--- a/stock_portfolio_report.xlsx
+++ b/stock_portfolio_report.xlsx
@@ -470,13 +470,13 @@
         <v>233673.2</v>
       </c>
       <c r="C2" t="n">
-        <v>258116.7500762939</v>
+        <v>256994.5010070801</v>
       </c>
       <c r="D2" t="n">
-        <v>24443.55007629396</v>
+        <v>23321.3010070801</v>
       </c>
       <c r="E2" t="n">
-        <v>10.46057060728144</v>
+        <v>9.980306259802193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BHEL, TATA CONSUMER AND RELIANCE PURCHASED
</commit_message>
<xml_diff>
--- a/stock_portfolio_report.xlsx
+++ b/stock_portfolio_report.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>233673.2</v>
+        <v>246169.15</v>
       </c>
       <c r="C2" t="n">
-        <v>253337.2521057129</v>
+        <v>265882.5480957031</v>
       </c>
       <c r="D2" t="n">
-        <v>19664.05210571291</v>
+        <v>19713.39809570313</v>
       </c>
       <c r="E2" t="n">
-        <v>8.415193571925625</v>
+        <v>8.00807009964617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>